<commit_message>
Leistungsdokument Thiemo Lachmund aktualisiert
</commit_message>
<xml_diff>
--- a/Leistungsdokumentation/Leistungsdokument -Thiemo Lachmund.xlsx
+++ b/Leistungsdokumentation/Leistungsdokument -Thiemo Lachmund.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\platy\Desktop\Studium\Software-Entwicklungsprojekt\gruppe06\Leistungsdokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{08ABEDA3-6C0E-4367-83D1-E179DE2DCB1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CEB40A-A597-49C5-A00B-88A8331134D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17860"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>Student:</t>
   </si>
@@ -130,12 +130,60 @@
   </si>
   <si>
     <t>22:30 Uhr</t>
+  </si>
+  <si>
+    <t>20 Uhr</t>
+  </si>
+  <si>
+    <t>21 Uhr</t>
+  </si>
+  <si>
+    <t>Exploding Kittens probespielen, Brainstorming zur Funktionsweise eines Bot</t>
+  </si>
+  <si>
+    <t>Grobes Konzept für schweren Bot im Kopf</t>
+  </si>
+  <si>
+    <t>12 Uhr</t>
+  </si>
+  <si>
+    <t>13:15 Uhr</t>
+  </si>
+  <si>
+    <t>Schriftliche Erarbeitung Konzept für leichten und schweren Bot</t>
+  </si>
+  <si>
+    <t>Abläufe für leichten und schweren Bot besprochen, ausgearbeitet und schriftlich festgehalten</t>
+  </si>
+  <si>
+    <t>Manuela</t>
+  </si>
+  <si>
+    <t>16:15 Uhr</t>
+  </si>
+  <si>
+    <t>Diagrammerstellung begonnen</t>
+  </si>
+  <si>
+    <t>9 Uhr</t>
+  </si>
+  <si>
+    <t>9:15 Uhr</t>
+  </si>
+  <si>
+    <t>Diagrammerstellung abgeschlossen</t>
+  </si>
+  <si>
+    <t>Diagramm für schweren Bot fertig</t>
+  </si>
+  <si>
+    <t>Diagramm für schweren Bot vorläufig fertig</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd&quot;.&quot;mm&quot;.&quot;yy"/>
     <numFmt numFmtId="165" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
@@ -185,7 +233,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -226,26 +274,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -258,12 +286,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -277,28 +304,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Heading" xfId="1"/>
-    <cellStyle name="Heading1" xfId="2"/>
-    <cellStyle name="Result" xfId="3"/>
-    <cellStyle name="Result2" xfId="4"/>
+    <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Heading1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Result" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Result2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -610,18 +626,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="14.1640625" customWidth="1"/>
     <col min="4" max="4" width="75.58203125" customWidth="1"/>
-    <col min="5" max="5" width="56.6640625" customWidth="1"/>
+    <col min="5" max="5" width="56.6640625" style="10" customWidth="1"/>
     <col min="6" max="6" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -649,7 +665,7 @@
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -657,239 +673,288 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>43944</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>43950</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>43951</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15">
+      <c r="A9" s="9">
         <v>43951</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15">
+      <c r="A10" s="9">
         <v>43955</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15">
+      <c r="A11" s="9">
         <v>43955</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="12"/>
+      <c r="A12" s="4">
+        <v>43972</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="12"/>
+      <c r="A13" s="4">
+        <v>43973</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="12"/>
+      <c r="A14" s="4">
+        <v>43973</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="12"/>
+      <c r="A15" s="4">
+        <v>43974</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="12"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="12"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="12"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="12"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="12"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="12"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="12"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="12"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="12"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="12"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39409448818897641" bottom="0.39409448818897641" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
@@ -898,7 +963,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -917,7 +982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>